<commit_message>
spaces removed from column name
</commit_message>
<xml_diff>
--- a/public/sample/Bulk Plans.xlsx
+++ b/public/sample/Bulk Plans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MERN Projects\stb-crm-project\stb-crm-backend\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BC40EF-2FA3-43B7-A3EC-8420A53F86F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA6B958-F4FD-452B-9B36-58644506A546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AA87AD8C-AD57-4B43-8B93-13222C870CF7}"/>
   </bookViews>
@@ -27,25 +27,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Plan Name</t>
-  </si>
-  <si>
     <t>MRP</t>
   </si>
   <si>
-    <t>LCO Price</t>
-  </si>
-  <si>
-    <t>BC Price</t>
-  </si>
-  <si>
-    <t>SD Count</t>
-  </si>
-  <si>
-    <t>HD Count</t>
-  </si>
-  <si>
     <t>MAHARASHTRA FTA 30d</t>
+  </si>
+  <si>
+    <t>PlanName</t>
+  </si>
+  <si>
+    <t>LCOPrice</t>
+  </si>
+  <si>
+    <t>BCPrice</t>
+  </si>
+  <si>
+    <t>SDCount</t>
+  </si>
+  <si>
+    <t>HDCount</t>
   </si>
 </sst>
 </file>
@@ -424,27 +424,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>153.4</v>

</xml_diff>